<commit_message>
add a xlsx creation feature
</commit_message>
<xml_diff>
--- a/test3.xlsx
+++ b/test3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>phone</t>
   </si>
@@ -25,34 +25,13 @@
     <t>overdue_days</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>guan.xiaojue@99cloud.net</t>
-  </si>
-  <si>
     <t>resources</t>
   </si>
   <si>
-    <t>project</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>默认</t>
-  </si>
-  <si>
-    <t>instance</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>test-instance1</t>
+    <t>邮件</t>
+  </si>
+  <si>
+    <t>还好</t>
   </si>
 </sst>
 </file>
@@ -384,13 +363,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,24 +377,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -423,63 +388,15 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="B5">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A4"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:B4"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>